<commit_message>
golden sky stories supplement
</commit_message>
<xml_diff>
--- a/golden-sky-stories/checklist.xlsx
+++ b/golden-sky-stories/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/golden-sky-stories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Source/japanese-collectors-list/golden-sky-stories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81110B3E-4E9E-CA42-BC6F-D8078273A331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8535B492-BEEC-2A4D-B927-655B1FF886FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="460" windowWidth="26740" windowHeight="15780" xr2:uid="{193A4FFC-09B8-A146-957E-37D85762A4A9}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="25480" windowHeight="15780" xr2:uid="{193A4FFC-09B8-A146-957E-37D85762A4A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>year</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>good_night.jpg</t>
+  </si>
+  <si>
+    <t>hometown_lane.jpg</t>
+  </si>
+  <si>
+    <t>Hometown Lane</t>
+  </si>
+  <si>
+    <t>ふるさとこみち</t>
   </si>
 </sst>
 </file>
@@ -463,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875ACC5E-7B3D-E941-BBBD-50661FEE1238}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,6 +626,26 @@
         <v>14</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2021</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F7">
     <sortCondition ref="A2:A7"/>

</xml_diff>